<commit_message>
add ENTER, more dd tests
</commit_message>
<xml_diff>
--- a/Data/Team_Name_Data.xlsx
+++ b/Data/Team_Name_Data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CS300-project\2 points\mattermost\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CS300-project\2 points\mattermost-duo-test\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,40 +24,43 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>team_name</t>
   </si>
   <si>
-    <t>TriThuYen</t>
-  </si>
-  <si>
-    <t>TriYenThu</t>
-  </si>
-  <si>
-    <t>ThuTriYen</t>
-  </si>
-  <si>
-    <t>ThuYenTri</t>
-  </si>
-  <si>
-    <t>YenTriThu</t>
-  </si>
-  <si>
-    <t>YenThuTri</t>
+    <t>Q1PQs0h9DL</t>
+  </si>
+  <si>
+    <t>gYsbx0Kffz</t>
+  </si>
+  <si>
+    <t>ZzgAYJtheg</t>
+  </si>
+  <si>
+    <t>OMupOkNokX</t>
+  </si>
+  <si>
+    <t>VOziCpR1mP</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -80,8 +83,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -362,10 +368,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -375,37 +381,33 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="4" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="5" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="6" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>